<commit_message>
Updated Part 1 Hand-In
</commit_message>
<xml_diff>
--- a/Part 1 - Algorithms with performance analysis/Computations.xlsx
+++ b/Part 1 - Algorithms with performance analysis/Computations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukad\Documents\GitHub\Mandelbrot-Mini-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukad\Documents\GitHub\Mandelbrot-Mini-Project\Part 1 - Algorithms with performance analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF7A3FE-48AC-49ED-AE34-25320C5037F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F568EBD1-FC95-4563-A2F1-365D6BF43BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77A506D2-D67E-4284-9023-358B7623300F}"/>
   </bookViews>
@@ -189,11 +189,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="da-DK"/>
+              <a:t>The</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK" baseline="0"/>
+              <a:t> 10 </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK"/>
               <a:t>Best Performing</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="da-DK" baseline="0"/>
-              <a:t> Parameters (top 10)</a:t>
+              <a:t> Parameters (Left lowest computation time)</a:t>
             </a:r>
             <a:endParaRPr lang="da-DK"/>
           </a:p>
@@ -261,10 +269,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Best Runs'!$A$2:$A$10</c:f>
+              <c:f>'Best Runs'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -290,6 +298,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -297,10 +308,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Best Runs'!$A$2:$A$10</c:f>
+              <c:f>'Best Runs'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -326,6 +337,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -363,10 +377,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Best Runs'!$A$2:$A$10</c:f>
+              <c:f>'Best Runs'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -392,6 +406,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -399,10 +416,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Best Runs'!$B$2:$B$10</c:f>
+              <c:f>'Best Runs'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>81</c:v>
                 </c:pt>
@@ -429,6 +446,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -480,12 +500,51 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Best Runs'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Best Runs'!$C$2:$C$10</c:f>
+              <c:f>'Best Runs'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.22848</c:v>
                 </c:pt>
@@ -512,6 +571,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.2623500000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.26936</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -866,6 +928,7 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -10021,9 +10084,9 @@
       <xdr:rowOff>173736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10595,7 +10658,7 @@
   <dimension ref="A1:C161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>